<commit_message>
final with installation files
</commit_message>
<xml_diff>
--- a/Data/PropStudy/510017 postBD.xlsx
+++ b/Data/PropStudy/510017 postBD.xlsx
@@ -1,15 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\OneDrive\Desktop\SeniorDesignFinal\Data\PropStudy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC4C36E-ADF4-43AB-AED4-FB88B82F8F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="19815" windowHeight="7890"/>
+    <workbookView xWindow="15360" yWindow="2010" windowWidth="13350" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="510017 postBD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -91,8 +107,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +636,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -666,7 +690,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,9 +722,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,6 +774,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -907,16 +967,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="N80" sqref="N80"/>
+    <sheetView tabSelected="1" topLeftCell="G66" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +1054,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3.2237268518518519E-2</v>
       </c>
@@ -1061,7 +1125,7 @@
         <v>231.38030000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3.2247685185185185E-2</v>
       </c>
@@ -1135,7 +1199,7 @@
         <v>242.9623</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3.2259259259259258E-2</v>
       </c>
@@ -1209,7 +1273,7 @@
         <v>324.66269999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.2269675925925924E-2</v>
       </c>
@@ -1283,7 +1347,7 @@
         <v>276.41590000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.2280092592592589E-2</v>
       </c>
@@ -1357,7 +1421,7 @@
         <v>399.834</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3.2302083333333335E-2</v>
       </c>
@@ -1431,7 +1495,7 @@
         <v>278.98070000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3.2314814814814817E-2</v>
       </c>
@@ -1505,7 +1569,7 @@
         <v>229.60130000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.2755787037037042E-2</v>
       </c>
@@ -1576,7 +1640,7 @@
         <v>1375.636</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3.2763888888888891E-2</v>
       </c>
@@ -1650,7 +1714,7 @@
         <v>1824.3869999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3.277199074074074E-2</v>
       </c>
@@ -1724,7 +1788,7 @@
         <v>4140.3850000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3.2778935185185189E-2</v>
       </c>
@@ -1798,7 +1862,7 @@
         <v>624.30370000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3.2788194444444446E-2</v>
       </c>
@@ -1872,7 +1936,7 @@
         <v>693.17129999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3.2798611111111105E-2</v>
       </c>
@@ -1946,7 +2010,7 @@
         <v>1111.51</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3.2809027777777777E-2</v>
       </c>
@@ -2020,7 +2084,7 @@
         <v>807.91390000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3.3081018518518517E-2</v>
       </c>
@@ -2091,7 +2155,7 @@
         <v>345.67160000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3.3092592592592597E-2</v>
       </c>
@@ -2165,7 +2229,7 @@
         <v>231.64439999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3.310648148148148E-2</v>
       </c>
@@ -2239,7 +2303,7 @@
         <v>195.43950000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3.3119212962962961E-2</v>
       </c>
@@ -2313,7 +2377,7 @@
         <v>172.13229999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3.3131944444444443E-2</v>
       </c>
@@ -2387,7 +2451,7 @@
         <v>254.89169999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3.3143518518518517E-2</v>
       </c>
@@ -2461,7 +2525,7 @@
         <v>224.81540000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3.3157407407407406E-2</v>
       </c>
@@ -2535,7 +2599,7 @@
         <v>248.56389999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3.3170138888888888E-2</v>
       </c>
@@ -2609,7 +2673,7 @@
         <v>241.1429</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3.318287037037037E-2</v>
       </c>
@@ -2683,7 +2747,7 @@
         <v>285.00749999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3.3194444444444443E-2</v>
       </c>
@@ -2757,7 +2821,7 @@
         <v>282.68470000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>3.3516203703703708E-2</v>
       </c>
@@ -2828,7 +2892,7 @@
         <v>259.91489999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3.3528935185185189E-2</v>
       </c>
@@ -2902,7 +2966,7 @@
         <v>266.41180000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3.3540509259259256E-2</v>
       </c>
@@ -2976,7 +3040,7 @@
         <v>227.61959999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>3.3553240740740745E-2</v>
       </c>
@@ -3050,7 +3114,7 @@
         <v>304.09190000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3.3565972222222219E-2</v>
       </c>
@@ -3124,7 +3188,7 @@
         <v>250.4837</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3.5010416666666662E-2</v>
       </c>
@@ -3195,7 +3259,7 @@
         <v>248.22640000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3.5021990740740742E-2</v>
       </c>
@@ -3269,7 +3333,7 @@
         <v>275.2869</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3.5035879629629632E-2</v>
       </c>
@@ -3343,7 +3407,7 @@
         <v>196.9751</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3.5049768518518515E-2</v>
       </c>
@@ -3417,7 +3481,7 @@
         <v>284.4248</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3.5061342592592595E-2</v>
       </c>
@@ -3491,7 +3555,7 @@
         <v>288.24579999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>3.5074074074074077E-2</v>
       </c>
@@ -3565,7 +3629,7 @@
         <v>196.38059999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3.5089120370370368E-2</v>
       </c>
@@ -3639,7 +3703,7 @@
         <v>221.89840000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3.5103009259259257E-2</v>
       </c>
@@ -3713,7 +3777,7 @@
         <v>199.35650000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3.5115740740740746E-2</v>
       </c>
@@ -3787,7 +3851,7 @@
         <v>305.28750000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>3.5126157407407405E-2</v>
       </c>
@@ -3861,7 +3925,7 @@
         <v>497.53840000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3.5135416666666662E-2</v>
       </c>
@@ -3935,7 +3999,7 @@
         <v>302.00990000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>3.5145833333333334E-2</v>
       </c>
@@ -4009,7 +4073,7 @@
         <v>347.30529999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3.5155092592592592E-2</v>
       </c>
@@ -4083,7 +4147,7 @@
         <v>273.91849999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>3.5166666666666666E-2</v>
       </c>
@@ -4157,7 +4221,7 @@
         <v>422.60789999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>3.5855324074074074E-2</v>
       </c>
@@ -4228,7 +4292,7 @@
         <v>218.91650000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3.5868055555555556E-2</v>
       </c>
@@ -4302,7 +4366,7 @@
         <v>194.78960000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3.5880787037037037E-2</v>
       </c>
@@ -4376,7 +4440,7 @@
         <v>247.8734</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3.5892361111111111E-2</v>
       </c>
@@ -4450,7 +4514,7 @@
         <v>240.98670000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>3.5905092592592593E-2</v>
       </c>
@@ -4524,7 +4588,7 @@
         <v>215.2885</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>3.5917824074074074E-2</v>
       </c>
@@ -4598,7 +4662,7 @@
         <v>174.2919</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>3.5930555555555556E-2</v>
       </c>
@@ -4672,7 +4736,7 @@
         <v>273.6841</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>3.5940972222222221E-2</v>
       </c>
@@ -4746,7 +4810,7 @@
         <v>342.60660000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>3.5952546296296302E-2</v>
       </c>
@@ -4820,7 +4884,7 @@
         <v>227.3098</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>3.5965277777777777E-2</v>
       </c>
@@ -4894,7 +4958,7 @@
         <v>213.96299999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>3.5979166666666666E-2</v>
       </c>
@@ -4968,7 +5032,7 @@
         <v>173.4734</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>3.753240740740741E-2</v>
       </c>
@@ -5039,7 +5103,7 @@
         <v>870.71079999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>3.7541666666666668E-2</v>
       </c>
@@ -5113,7 +5177,7 @@
         <v>478.2509</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>3.7550925925925925E-2</v>
       </c>
@@ -5187,7 +5251,7 @@
         <v>463.80849999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>3.7560185185185183E-2</v>
       </c>
@@ -5261,7 +5325,7 @@
         <v>637.4357</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>3.7569444444444447E-2</v>
       </c>
@@ -5335,7 +5399,7 @@
         <v>444.03899999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>3.7591435185185186E-2</v>
       </c>
@@ -5409,7 +5473,7 @@
         <v>313.8116</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>3.7612268518518517E-2</v>
       </c>
@@ -5483,7 +5547,7 @@
         <v>263.22739999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>3.7623842592592598E-2</v>
       </c>
@@ -5557,7 +5621,7 @@
         <v>219.9742</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>3.7635416666666664E-2</v>
       </c>
@@ -5631,7 +5695,7 @@
         <v>310.32769999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>3.764583333333333E-2</v>
       </c>
@@ -5705,7 +5769,7 @@
         <v>311.13580000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>3.765740740740741E-2</v>
       </c>
@@ -5779,7 +5843,7 @@
         <v>220.3424</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>3.7670138888888885E-2</v>
       </c>
@@ -5853,7 +5917,7 @@
         <v>190.4984</v>
       </c>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>3.7682870370370374E-2</v>
       </c>
@@ -5927,7 +5991,7 @@
         <v>262.83589999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>3.7694444444444447E-2</v>
       </c>
@@ -6001,7 +6065,7 @@
         <v>429.80200000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>3.7703703703703705E-2</v>
       </c>
@@ -6075,7 +6139,7 @@
         <v>823.02430000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>3.7711805555555554E-2</v>
       </c>
@@ -6149,7 +6213,7 @@
         <v>543.9914</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>3.7721064814814818E-2</v>
       </c>
@@ -6223,7 +6287,7 @@
         <v>445.94799999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>3.7730324074074069E-2</v>
       </c>
@@ -6297,7 +6361,7 @@
         <v>1001.277</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>3.7739583333333333E-2</v>
       </c>
@@ -6371,7 +6435,7 @@
         <v>509.02100000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>3.7748842592592598E-2</v>
       </c>
@@ -6445,11 +6509,15 @@
         <v>339.5111</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D77">
         <f>AVERAGE(D2:D75)</f>
         <v>30.328725364864862</v>
       </c>
+      <c r="L77">
+        <f>AVERAGE(L1:L75)</f>
+        <v>0.34330256891891903</v>
+      </c>
       <c r="M77">
         <f>AVERAGE(M2:M75)</f>
         <v>62.656178243243247</v>
@@ -6457,6 +6525,24 @@
       <c r="S77">
         <f>AVERAGE(S2:S75)</f>
         <v>0.48887942432432435</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f>_xlfn.STDEV.S(D2:D75)</f>
+        <v>8.6071270904696</v>
+      </c>
+      <c r="L78">
+        <f>_xlfn.STDEV.S(L2:L75)</f>
+        <v>5.9605996967572315E-2</v>
+      </c>
+      <c r="M78">
+        <f>_xlfn.STDEV.S(M1:M75)</f>
+        <v>10.449111353899715</v>
+      </c>
+      <c r="S78">
+        <f>_xlfn.STDEV.S(S1:S75)</f>
+        <v>2.8234306928089044E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>